<commit_message>
rework of extraction to propagate errors.
</commit_message>
<xml_diff>
--- a/backend/fms_core/static/submission_templates/Sample_update_v0.6.xlsx
+++ b/backend/fms_core/static/submission_templates/Sample_update_v0.6.xlsx
@@ -1534,7 +1534,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="18.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="21.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.27"/>
   </cols>
   <sheetData>
@@ -6578,17 +6578,17 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G8:G391" type="list">
-      <formula1>"YES"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
     <dataValidation allowBlank="true" operator="between" promptTitle="Coordinate" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C8:C391" type="list">
       <formula1>Index!$B$2:$B$385</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="false" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H8:H391" type="none">
-      <formula1>1899-12-30</formula1>
-      <formula2>1899-12-30</formula2>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="G8:G391" type="list">
+      <formula1>"YES,NO"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="H8:H391" type="none">
+      <formula1>0</formula1>
+      <formula2>0</formula2>
     </dataValidation>
   </dataValidations>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>